<commit_message>
Updated Product Backlog and Added New Use Cases.
Product backlog has been updated to current working file.

Change Current Location and Check Historical Weather Use Cases have been added to the use case documentation folder.
</commit_message>
<xml_diff>
--- a/documentation/DevOps - Product Backlog.xlsx
+++ b/documentation/DevOps - Product Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Priority</t>
   </si>
@@ -25,6 +25,15 @@
     <t>Why</t>
   </si>
   <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
     <t>As the user</t>
   </si>
   <si>
@@ -34,6 +43,9 @@
     <t>So that I can be informed of the current weather in a given location</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>check warnings (severe weather, air quality, etc)</t>
   </si>
   <si>
@@ -46,10 +58,10 @@
     <t>So that I can be more precisely informed of the weather</t>
   </si>
   <si>
-    <t>check future weather for given location</t>
-  </si>
-  <si>
-    <t>So that I can be informed of the weather in the future</t>
+    <t>partial (daily only)</t>
+  </si>
+  <si>
+    <t>partial (hourly only)</t>
   </si>
   <si>
     <t>save locations for future weather checking</t>
@@ -58,22 +70,73 @@
     <t>So that I can be informed of weather in specific areas</t>
   </si>
   <si>
-    <t>check local events (concerts, marathon, etc.)</t>
-  </si>
-  <si>
-    <t>So that I can be informed of events happening in a given location</t>
-  </si>
-  <si>
     <t>check a weather map based on given location</t>
   </si>
   <si>
     <t>So that I can be informed over a broader range of locations</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>as the user</t>
+  </si>
+  <si>
+    <t>search weather locations nearest me</t>
+  </si>
+  <si>
+    <t>So that I can get information for weather locations near me easier</t>
+  </si>
+  <si>
     <t>check previous weather for given location</t>
   </si>
   <si>
     <t>So I can be informed of previous weather trends</t>
+  </si>
+  <si>
+    <t>have the option to maximize the application window</t>
+  </si>
+  <si>
+    <t>So I can see the information in a bigger window</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>change current location manually</t>
+  </si>
+  <si>
+    <t>So that i can get information pertaining to my location if IP based is not working</t>
+  </si>
+  <si>
+    <t>Next Steps:</t>
+  </si>
+  <si>
+    <t>Wireframe</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Use cases and diagram</t>
+  </si>
+  <si>
+    <t>Start system design</t>
+  </si>
+  <si>
+    <t>sprint backlog</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>moved</t>
   </si>
 </sst>
 </file>
@@ -99,9 +162,11 @@
     <font>
       <b/>
       <i/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +179,12 @@
         <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -121,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -131,10 +202,17 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -355,8 +433,9 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="41.29"/>
     <col customWidth="1" min="3" max="3" width="63.0"/>
-    <col customWidth="1" min="4" max="4" width="78.71"/>
-    <col customWidth="1" min="5" max="5" width="15.71"/>
+    <col customWidth="1" min="4" max="4" width="105.43"/>
+    <col customWidth="1" min="5" max="5" width="16.0"/>
+    <col customWidth="1" min="6" max="6" width="17.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -372,121 +451,266 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
         <v>1.0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>